<commit_message>
Changed view of basic details in show page, made it
Changed view of basic details in show page, made it better.
Added functionality to edit the basic details of student.
</commit_message>
<xml_diff>
--- a/uploads/Exam Fee dummy.xlsx
+++ b/uploads/Exam Fee dummy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalak\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\versatile\Desktop\test excel sheet fyproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7815" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -169,6 +169,10 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +456,13 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="22" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -485,7 +492,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -541,7 +548,7 @@
       <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>150160702013</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -595,7 +602,7 @@
       <c r="I3" s="1">
         <v>2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <v>150160702013</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -648,7 +655,7 @@
       <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>150160702013</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -701,7 +708,7 @@
       <c r="I5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>150160702013</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -754,7 +761,7 @@
       <c r="I6" s="1">
         <v>5</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>150160702013</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -807,7 +814,7 @@
       <c r="I7" s="1">
         <v>6</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>150160702013</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -860,7 +867,7 @@
       <c r="I8" s="1">
         <v>7</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>150160702013</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -913,7 +920,7 @@
       <c r="I9" s="1">
         <v>8</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>150160702013</v>
       </c>
       <c r="K9" s="1" t="s">

</xml_diff>